<commit_message>
aded a demo for c, r, s
</commit_message>
<xml_diff>
--- a/main/files(example folder)/test-5-diferent.xlsx
+++ b/main/files(example folder)/test-5-diferent.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\python&amp;excel\data-search-with-python\main\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\python&amp;excel\data-search-with-python\main\files(example folder)\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -398,7 +398,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,7 +519,6 @@
         <v>81</v>
       </c>
       <c r="E7">
-        <f>SUM(E2:E6)/5</f>
         <v>87.2</v>
       </c>
     </row>

</xml_diff>